<commit_message>
drafts clean_data.R, makes changes to medatada field names
</commit_message>
<xml_diff>
--- a/data-raw/metadata/feather_metadata.xlsx
+++ b/data-raw/metadata/feather_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\edi-feather-snorkel\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7252FF89-1163-4D3C-809C-696D79BF0243}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8E6BAB2-8437-4CBD-BE73-56BA3DB5E0B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5130" yWindow="840" windowWidth="18240" windowHeight="13890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="63">
   <si>
     <t>name</t>
   </si>
@@ -85,12 +85,6 @@
     <t>fall run</t>
   </si>
   <si>
-    <t>trap</t>
-  </si>
-  <si>
-    <t>catch</t>
-  </si>
-  <si>
     <t>juvenile production estimate</t>
   </si>
   <si>
@@ -148,9 +142,6 @@
     <t>ongoing</t>
   </si>
   <si>
-    <t>monthly</t>
-  </si>
-  <si>
     <t>geographic_description</t>
   </si>
   <si>
@@ -224,6 +215,9 @@
   </si>
   <si>
     <t>Snorkel surveying of juvenile Chinook salmon the Feather River</t>
+  </si>
+  <si>
+    <t>annually</t>
   </si>
 </sst>
 </file>
@@ -579,8 +573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -598,7 +592,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -614,45 +608,45 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" t="s">
         <v>48</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>49</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>50</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>51</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>52</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>53</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>54</v>
-      </c>
-      <c r="H1" t="s">
-        <v>55</v>
-      </c>
-      <c r="I1" t="s">
-        <v>56</v>
-      </c>
-      <c r="J1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -666,7 +660,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -693,13 +687,13 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
@@ -722,7 +716,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -737,10 +731,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -751,10 +745,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -795,16 +789,6 @@
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -823,24 +807,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
         <v>24</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>25</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>26</v>
-      </c>
-      <c r="D1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -881,13 +865,13 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
@@ -915,22 +899,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
         <v>30</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>31</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>32</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>33</v>
-      </c>
-      <c r="E1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F1" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -943,24 +927,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -973,36 +959,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="6" max="7" width="17.81640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
         <v>40</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>41</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>42</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>43</v>
-      </c>
-      <c r="E1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B2">
         <v>-121.63263600000001</v>
@@ -1017,7 +1008,7 @@
         <v>39.212150000000001</v>
       </c>
       <c r="F2" s="1">
-        <v>35786</v>
+        <v>36516</v>
       </c>
       <c r="G2" s="1">
         <v>45337</v>

</xml_diff>

<commit_message>
changes domains in metadata
</commit_message>
<xml_diff>
--- a/data-raw/metadata/feather_metadata.xlsx
+++ b/data-raw/metadata/feather_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\edi-feather-snorkel\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8E6BAB2-8437-4CBD-BE73-56BA3DB5E0B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1631628-BD60-42B3-A533-386942A41298}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="1" r:id="rId1"/>
@@ -241,12 +241,10 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -266,17 +264,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -574,7 +571,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -608,7 +605,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -660,7 +657,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -703,9 +700,6 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{EBA16962-CF64-4CE6-9C97-8E652015DEEF}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
@@ -748,7 +742,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -801,7 +795,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -822,12 +818,17 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="A2" xr:uid="{98AFD1B8-FD6A-4EC6-9E7B-E4E67F57B552}">
+      <formula1>"CCO,CCBY"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
@@ -837,8 +838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -881,9 +882,6 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{A80D5799-12E8-40E4-8758-6BBB3A99EFA6}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>

<commit_message>
updates methods and rewrites metadata
</commit_message>
<xml_diff>
--- a/data-raw/metadata/feather_metadata.xlsx
+++ b/data-raw/metadata/feather_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\edi-feather-snorkel\data-raw\metadata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erincain/Documents/Git/edi-feather-snorkel/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1631628-BD60-42B3-A533-386942A41298}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE4018B5-1F3A-0C47-8B25-2044B64BC9C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25820" windowHeight="15500" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="63">
   <si>
     <t>name</t>
   </si>
@@ -79,15 +79,6 @@
     <t>keywordThesaurus</t>
   </si>
   <si>
-    <t>spring run</t>
-  </si>
-  <si>
-    <t>fall run</t>
-  </si>
-  <si>
-    <t>juvenile production estimate</t>
-  </si>
-  <si>
     <t>Oncorhynchus tshawytscha</t>
   </si>
   <si>
@@ -202,9 +193,6 @@
     <t>Feather Snorkel Survey</t>
   </si>
   <si>
-    <t>Snorkel Data Feather River</t>
-  </si>
-  <si>
     <t>Casey</t>
   </si>
   <si>
@@ -218,6 +206,18 @@
   </si>
   <si>
     <t>annually</t>
+  </si>
+  <si>
+    <t>Distribution and habitat use of juvenile Feather River salmonids</t>
+  </si>
+  <si>
+    <t>habitat</t>
+  </si>
+  <si>
+    <t>Feather River</t>
+  </si>
+  <si>
+    <t>steelhead</t>
   </si>
 </sst>
 </file>
@@ -227,7 +227,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -244,6 +244,12 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -270,8 +276,8 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -574,9 +580,9 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -587,9 +593,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -603,47 +609,54 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" t="s">
         <v>45</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>46</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>47</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>48</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>49</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>50</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>51</v>
       </c>
-      <c r="H1" t="s">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>52</v>
       </c>
-      <c r="I1" t="s">
-        <v>53</v>
-      </c>
-      <c r="J1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>55</v>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -660,9 +673,9 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -682,15 +695,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>60</v>
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
+        <v>56</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
@@ -710,12 +723,16 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="23.83203125" customWidth="1"/>
+    <col min="2" max="2" width="27.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -723,12 +740,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>57</v>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -742,12 +759,15 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -755,34 +775,34 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -799,28 +819,28 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
         <v>22</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>23</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="D1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -838,13 +858,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -864,15 +884,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>60</v>
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
+        <v>56</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
@@ -893,26 +913,26 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
         <v>28</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>29</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>30</v>
-      </c>
-      <c r="D1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F1" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -929,22 +949,22 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -961,37 +981,37 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="7" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="17.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" t="s">
         <v>37</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>38</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>39</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>40</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>41</v>
-      </c>
-      <c r="F1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>44</v>
       </c>
       <c r="B2">
         <v>-121.63263600000001</v>

</xml_diff>